<commit_message>
me faltaron unas cositas, todavia no he terminado :(
</commit_message>
<xml_diff>
--- a/docs/traceability.xlsx
+++ b/docs/traceability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo Ramos\Desktop\Lab2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8411F3-8518-4097-B73E-AFF72EE01070}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661B21BD-2616-4A1E-AB9D-ECCB1D569FA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE15EB1C-EB24-48A5-8842-F2494A017B9A}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{FE15EB1C-EB24-48A5-8842-F2494A017B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -60,18 +60,12 @@
     <t>enterDate():GregorianCalendar</t>
   </si>
   <si>
-    <t>registerClient(name : String, crn : int, date : GregorianCalendar, typeClient : int) : String</t>
-  </si>
-  <si>
     <t>searchClient(crn : int) : Client</t>
   </si>
   <si>
     <t>getPositionEmpty(array : Client[]) : int</t>
   </si>
   <si>
-    <t>Client(name : String, crn : int, date : GregorianCalendar, typeClient : int)</t>
-  </si>
-  <si>
     <t>Client</t>
   </si>
   <si>
@@ -205,6 +199,12 @@
   </si>
   <si>
     <t>lookForSpace() : boolean</t>
+  </si>
+  <si>
+    <t>registerClient(name : String, crn : int, date : GregorianCalendar) : String</t>
+  </si>
+  <si>
+    <t>Client(name : String, crn : int, date : GregorianCalendar)</t>
   </si>
 </sst>
 </file>
@@ -419,6 +419,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,31 +443,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -772,7 +772,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,10 +793,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -804,401 +804,415 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="7" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="22" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
+      <c r="B22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20" t="s">
+      <c r="C23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="C25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="2" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="23"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>43</v>
+      <c r="A30" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="22"/>
+      <c r="B32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="22"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="4" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="22"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="22"/>
+      <c r="B35" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="4" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="23"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="3" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="21" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>47</v>
+      <c r="A40" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="22"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="4" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="22"/>
+      <c r="B43" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="4" t="s">
+      <c r="B45" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
-      <c r="B46" s="19"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="22"/>
+      <c r="B48" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="22"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="4" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="23"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="6" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="17"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A22"/>
@@ -1207,20 +1221,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>